<commit_message>
Use blank row to mark end of data
</commit_message>
<xml_diff>
--- a/test/resources/book_a.xlsx
+++ b/test/resources/book_a.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hale/Documents/HGSC/costing/software/pipexl/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5641DE7-DF80-6E47-80F8-4C58703C623B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23BC7CD-EDFE-D243-AA07-945F7D91D7CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{BFA5E035-CBCD-C141-B2A6-5392F69D791A}"/>
+    <workbookView xWindow="1300" yWindow="7480" windowWidth="29380" windowHeight="18760" xr2:uid="{4430D184-CDCD-B943-BB5D-99174887BC65}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_a" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>param1</t>
   </si>
@@ -39,6 +39,12 @@
     <t>table_marker</t>
   </si>
   <si>
+    <t>sep</t>
+  </si>
+  <si>
+    <t>exclude_b</t>
+  </si>
+  <si>
     <t>exclude_a</t>
   </si>
   <si>
@@ -57,112 +63,136 @@
     <t>value_c</t>
   </si>
   <si>
-    <t>sep</t>
-  </si>
-  <si>
-    <t>exclude_b</t>
+    <t>other_a</t>
+  </si>
+  <si>
+    <t>other_b</t>
+  </si>
+  <si>
+    <t>other_c</t>
+  </si>
+  <si>
+    <t>SO 1 Qp</t>
+  </si>
+  <si>
+    <t>h6 6 hT</t>
+  </si>
+  <si>
+    <t>Ww 5 zh</t>
+  </si>
+  <si>
+    <t>mz 5 0z</t>
+  </si>
+  <si>
+    <t>5F 3 gG</t>
+  </si>
+  <si>
+    <t>oL 2 RJ</t>
+  </si>
+  <si>
+    <t>8x 5 Mh</t>
+  </si>
+  <si>
+    <t>iI 4 lb</t>
+  </si>
+  <si>
+    <t>g6 1 3a</t>
+  </si>
+  <si>
+    <t>Zh 2 B1</t>
+  </si>
+  <si>
+    <t>unit food held</t>
+  </si>
+  <si>
+    <t>taste strange written</t>
+  </si>
+  <si>
+    <t>sound rolled table</t>
+  </si>
+  <si>
+    <t>help slowly crowd</t>
+  </si>
+  <si>
+    <t>because week were</t>
+  </si>
+  <si>
+    <t>agree million soon</t>
+  </si>
+  <si>
+    <t>Africa neighbor French</t>
+  </si>
+  <si>
+    <t>unit each eggs</t>
+  </si>
+  <si>
+    <t>mile best hard</t>
+  </si>
+  <si>
+    <t>steel were planet</t>
+  </si>
+  <si>
+    <t>Jamaica move uncle</t>
+  </si>
+  <si>
+    <t>century warm center</t>
+  </si>
+  <si>
+    <t>himself shirt lake</t>
+  </si>
+  <si>
+    <t>told vowel bell</t>
+  </si>
+  <si>
+    <t>pain discover total</t>
+  </si>
+  <si>
+    <t>silent southern receive</t>
   </si>
   <si>
     <t>doctor borrow seem</t>
   </si>
   <si>
-    <t>unit food held</t>
-  </si>
-  <si>
-    <t>Africa neighbor French</t>
-  </si>
-  <si>
-    <t>SO 1 Qp</t>
-  </si>
-  <si>
     <t>Damascus case small</t>
   </si>
   <si>
-    <t>taste strange written</t>
-  </si>
-  <si>
-    <t>unit each eggs</t>
-  </si>
-  <si>
-    <t>h6 6 hT</t>
-  </si>
-  <si>
-    <t>mile best hard</t>
-  </si>
-  <si>
-    <t>Ww 5 zh</t>
+    <t>hunt lead once</t>
+  </si>
+  <si>
+    <t>soft send tore</t>
+  </si>
+  <si>
+    <t>hill gather major</t>
+  </si>
+  <si>
+    <t>exciting device pleasant</t>
+  </si>
+  <si>
+    <t>school signal easy</t>
+  </si>
+  <si>
+    <t>horse strike equal</t>
+  </si>
+  <si>
+    <t>health region away</t>
+  </si>
+  <si>
+    <t>remember change fair</t>
+  </si>
+  <si>
+    <t>soil cells inch</t>
+  </si>
+  <si>
+    <t>scene still wire</t>
+  </si>
+  <si>
+    <t>prepare spell left</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>hunt lead once</t>
-  </si>
-  <si>
-    <t>sound rolled table</t>
-  </si>
-  <si>
-    <t>steel were planet</t>
-  </si>
-  <si>
-    <t>mz 5 0z</t>
-  </si>
-  <si>
-    <t>soft send tore</t>
-  </si>
-  <si>
-    <t>help slowly crowd</t>
-  </si>
-  <si>
-    <t>Jamaica move uncle</t>
-  </si>
-  <si>
-    <t>5F 3 gG</t>
-  </si>
-  <si>
-    <t>hill gather major</t>
-  </si>
-  <si>
-    <t>because week were</t>
-  </si>
-  <si>
-    <t>century warm center</t>
-  </si>
-  <si>
-    <t>oL 2 RJ</t>
-  </si>
-  <si>
-    <t>himself shirt lake</t>
-  </si>
-  <si>
-    <t>8x 5 Mh</t>
-  </si>
-  <si>
-    <t>told vowel bell</t>
-  </si>
-  <si>
-    <t>iI 4 lb</t>
-  </si>
-  <si>
-    <t>exciting device pleasant</t>
-  </si>
-  <si>
-    <t>pain discover total</t>
-  </si>
-  <si>
-    <t>g6 1 3a</t>
-  </si>
-  <si>
-    <t>school signal easy</t>
-  </si>
-  <si>
-    <t>agree million soon</t>
-  </si>
-  <si>
-    <t>silent southern receive</t>
-  </si>
-  <si>
-    <t>Zh 2 B1</t>
+    <t>fini</t>
   </si>
 </sst>
 </file>
@@ -203,10 +233,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -521,11 +551,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701381AB-789B-0F4E-BA82-4CEA31D2C932}">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAB6BE0-37F5-564A-875D-B30D55CC50FD}">
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,34 +599,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1">
+        <v>43466</v>
+      </c>
+      <c r="I6" s="1">
+        <v>43497</v>
+      </c>
+      <c r="J6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="K6" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2">
-        <v>43466</v>
-      </c>
-      <c r="I6" s="2">
-        <v>43497</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -604,16 +634,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3">
         <v>79.819999999999993</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -634,19 +664,19 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3">
         <v>19.98</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3">
         <v>49.81</v>
@@ -669,13 +699,13 @@
         <v>55.19</v>
       </c>
       <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
         <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
       </c>
       <c r="G9" s="3">
         <v>37.22</v>
@@ -690,20 +720,20 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3">
         <f>C8+C9</f>
         <v>75.17</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" ref="G10:I10" si="0">G8+G9</f>
@@ -723,19 +753,19 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3">
         <v>77.52</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G11" s="3">
         <v>75.98</v>
@@ -753,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3">
         <v>29.61</v>
@@ -762,10 +792,10 @@
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G12" s="3">
         <v>87.71</v>
@@ -781,19 +811,19 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3">
         <v>90.3</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G13" s="3">
         <v>27</v>
@@ -814,13 +844,13 @@
         <v>19.16</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G14" s="3">
         <v>8.3800000000000008</v>
@@ -841,13 +871,13 @@
         <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G15" s="3">
         <v>70.06</v>
@@ -865,19 +895,19 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3">
         <v>8.48</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="G16" s="3">
         <v>47.72</v>
@@ -890,20 +920,20 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C17" s="3">
         <f>C13+C14+C15+C16</f>
         <v>201.93999999999997</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" ref="G17:I17" si="1">G13+G14+G15+G16</f>
@@ -923,19 +953,19 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3">
         <v>89.74</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="G18" s="3">
         <v>61.73</v>
@@ -948,6 +978,55 @@
       </c>
       <c r="K18" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RecordSet.sum_by handles case of summable key
</commit_message>
<xml_diff>
--- a/test/resources/book_a.xlsx
+++ b/test/resources/book_a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hale/Documents/HGSC/costing/software/pipexl/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49461AAB-A047-644F-A16E-791365918808}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F686C13C-A991-6348-B6D7-18AEB60DAD48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="7480" windowWidth="29380" windowHeight="20060" xr2:uid="{4430D184-CDCD-B943-BB5D-99174887BC65}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
   <si>
     <t>param1</t>
   </si>
@@ -329,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -349,6 +349,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAB6BE0-37F5-564A-875D-B30D55CC50FD}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1041,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1074,7 +1077,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1107,12 +1110,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>10</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C22">
         <v>8</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>13</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>21</v>
       </c>
@@ -1156,12 +1159,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D28" s="13" t="s">
         <v>7</v>
       </c>
@@ -1177,8 +1180,20 @@
       <c r="H28" s="14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D29" s="15" t="s">
         <v>23</v>
       </c>
@@ -1194,8 +1209,20 @@
       <c r="H29" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D30" s="15" t="s">
         <v>23</v>
       </c>
@@ -1211,8 +1238,20 @@
       <c r="H30" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>2</v>
+      </c>
+      <c r="P30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D31" s="15" t="s">
         <v>23</v>
       </c>
@@ -1228,8 +1267,20 @@
         <f>H29+H30</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="O31">
+        <v>3</v>
+      </c>
+      <c r="P31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D32" s="15" t="s">
         <v>24</v>
       </c>
@@ -1245,8 +1296,14 @@
       <c r="H32" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D33" s="15" t="s">
         <v>24</v>
       </c>
@@ -1262,8 +1319,14 @@
       <c r="H33" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D34" s="15" t="s">
         <v>24</v>
       </c>
@@ -1279,8 +1342,14 @@
       <c r="H34" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D35" s="15" t="s">
         <v>24</v>
       </c>
@@ -1298,8 +1367,14 @@
         <f>H32+H33+H34</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D36" s="15" t="s">
         <v>25</v>
       </c>
@@ -1315,8 +1390,14 @@
       <c r="H36" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D37" s="15" t="s">
         <v>25</v>
       </c>
@@ -1332,8 +1413,14 @@
       <c r="H37" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D38" s="15" t="s">
         <v>25</v>
       </c>
@@ -1349,8 +1436,14 @@
         <f>H36+H37</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <v>2</v>
+      </c>
+      <c r="M38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D39" s="15" t="s">
         <v>26</v>
       </c>
@@ -1366,8 +1459,14 @@
       <c r="H39" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D40" s="15" t="s">
         <v>27</v>
       </c>
@@ -1383,8 +1482,14 @@
       <c r="H40" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <v>2</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D41" s="15" t="s">
         <v>27</v>
       </c>
@@ -1400,8 +1505,14 @@
       <c r="H41" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>3</v>
+      </c>
+      <c r="M41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D42" s="15" t="s">
         <v>27</v>
       </c>
@@ -1418,7 +1529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D43" s="15" t="s">
         <v>27</v>
       </c>
@@ -1435,7 +1546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D44" s="15" t="s">
         <v>27</v>
       </c>
@@ -1452,7 +1563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="4:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D45" s="16" t="s">
         <v>28</v>
       </c>
@@ -1470,6 +1581,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="N29:O45">
+    <sortCondition ref="N29:N45"/>
+    <sortCondition ref="O29:O45"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>